<commit_message>
Updated: code/deformable-protopnet/image_retrieval_utilities.py, code/deformable-protopnet/models_counterfactuals_retrieval.py, cub2002011_counterfactual_retrieval.sh, paper/paper_protostats_results.xlsx
</commit_message>
<xml_diff>
--- a/paper/paper_protostats_results.xlsx
+++ b/paper/paper_protostats_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tiagofilipesousagoncalves/Desktop/GitHub/proto-counterfactuals/paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D51132E7-D45A-9D42-BC23-6DB5DB2B0566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A8E5CB-1E34-B243-9FB6-374CB4E2517F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="33">
   <si>
     <t>ProtoPNet</t>
   </si>
@@ -113,6 +113,15 @@
   </si>
   <si>
     <t>Average # Prototypes / Class Identity</t>
+  </si>
+  <si>
+    <t>2023-01-09_01-07-48</t>
+  </si>
+  <si>
+    <t>2023-01-11_18-27-35</t>
+  </si>
+  <si>
+    <t>2023-01-13_07-25-59</t>
   </si>
 </sst>
 </file>
@@ -120,7 +129,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -167,10 +176,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -180,6 +186,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -460,7 +469,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -469,23 +478,23 @@
     <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="29.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="4" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -512,143 +521,173 @@
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="6">
         <v>1.6182374957468499</v>
       </c>
       <c r="D3" s="3"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6" t="s">
+      <c r="E3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>5</v>
+      </c>
+      <c r="G3" s="6">
+        <v>6.8878787878787797</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="3"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6" t="s">
+      <c r="E4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>7</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="6">
         <v>1.9719298245614001</v>
       </c>
       <c r="D5" s="3"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6" t="s">
+      <c r="E5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>9</v>
+      </c>
+      <c r="G5" s="6">
+        <v>4.2010796221322497</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="3"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6" t="s">
+      <c r="E6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>10</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <v>3.73062694704049</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6" t="s">
+      <c r="E7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>12</v>
+      </c>
+      <c r="G7" s="6">
+        <v>9.4899871756930008</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="3"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6" t="s">
+      <c r="E8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>13</v>
       </c>
+      <c r="G8" s="6" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
@@ -666,7 +705,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -680,17 +719,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="4" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -717,20 +756,20 @@
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="6">
         <v>7.8866279069767398</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="6">
         <v>9.8805194805194798</v>
       </c>
     </row>
@@ -738,20 +777,20 @@
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="6" t="s">
         <v>6</v>
       </c>
     </row>
@@ -759,20 +798,20 @@
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="6">
         <v>7.3470588235294096</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="6">
         <v>9.9474940334128803</v>
       </c>
     </row>
@@ -780,20 +819,20 @@
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="6" t="s">
         <v>6</v>
       </c>
     </row>
@@ -801,20 +840,20 @@
       <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <v>9.3294392523364493</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="6">
         <v>8</v>
       </c>
     </row>
@@ -822,68 +861,68 @@
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
@@ -901,7 +940,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -916,17 +955,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="4" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -953,20 +992,20 @@
       <c r="A3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="6">
         <v>8.99166666666666</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="6">
         <v>9.5724137931034399</v>
       </c>
     </row>
@@ -974,20 +1013,20 @@
       <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="6">
         <v>8.4020618556700999</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="6" t="s">
         <v>6</v>
       </c>
     </row>
@@ -995,20 +1034,20 @@
       <c r="A5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="6">
         <v>9.4672897196261605</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="6">
         <v>9.5957446808510607</v>
       </c>
     </row>
@@ -1016,20 +1055,20 @@
       <c r="A6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6">
         <v>6.7916666666666599</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="6" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1037,20 +1076,20 @@
       <c r="A7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <v>6.76</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="6">
         <v>9.8681318681318597</v>
       </c>
     </row>
@@ -1058,68 +1097,68 @@
       <c r="A8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="6">
         <v>5.8216216216216203</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
@@ -1137,7 +1176,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1152,17 +1191,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="4" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -1186,116 +1225,116 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6" t="s">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="3"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6" t="s">
+      <c r="E3" s="5"/>
+      <c r="F3" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6" t="s">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="3"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6" t="s">
+      <c r="E4" s="5"/>
+      <c r="F4" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6" t="s">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="3"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6" t="s">
+      <c r="E5" s="5"/>
+      <c r="F5" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6" t="s">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="3"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6" t="s">
+      <c r="E6" s="5"/>
+      <c r="F6" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6" t="s">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6" t="s">
+      <c r="E7" s="5"/>
+      <c r="F7" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6" t="s">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="3"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6" t="s">
+      <c r="E8" s="5"/>
+      <c r="F8" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>

</xml_diff>